<commit_message>
starting 19, saved 143 notes
</commit_message>
<xml_diff>
--- a/0 NeetCode/143. Reorder List/Whiteboards/Solution.xlsx
+++ b/0 NeetCode/143. Reorder List/Whiteboards/Solution.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\0 NeetCode\143. Reorder List\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFCF212C-B0A5-4378-A9A6-D07F29ABB000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F8FABC-B808-45AB-AF37-0404E67E99E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Reverrse" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,9 +36,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="10">
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Np</t>
+  </si>
+  <si>
+    <t>c=n</t>
+  </si>
+  <si>
+    <t>p=c</t>
+  </si>
+  <si>
+    <t>1p</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>z</t>
   </si>
 </sst>
 </file>
@@ -392,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="E9:AK22"/>
+  <dimension ref="E9:AM30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="AF17" sqref="AF17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -403,7 +431,7 @@
     <col min="1" max="16384" width="4.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="5:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E9" s="1">
         <v>1</v>
       </c>
@@ -465,7 +493,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="5:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E10" s="1">
         <v>2</v>
       </c>
@@ -527,7 +555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="5:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AF12" s="1">
         <v>1</v>
       </c>
@@ -547,7 +575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="5:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R14" s="1">
         <v>1</v>
       </c>
@@ -578,19 +606,37 @@
       <c r="AH14" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="5:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AK14" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL14" s="1">
+        <v>5</v>
+      </c>
+      <c r="AM14" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AF15" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AG15" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AH15" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="5:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AK15" s="1">
+        <v>5</v>
+      </c>
+      <c r="AL15" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM15" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R16" s="1">
         <v>1</v>
       </c>
@@ -603,8 +649,11 @@
       <c r="U16" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="18:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="18:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R17" s="1">
         <v>7</v>
       </c>
@@ -614,8 +663,11 @@
       <c r="T17" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="18:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF17" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="18:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R22" s="1">
         <v>1</v>
       </c>
@@ -636,6 +688,529 @@
       </c>
       <c r="X22" s="1">
         <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="18:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R26" s="1">
+        <v>1</v>
+      </c>
+      <c r="S26" s="1">
+        <v>2</v>
+      </c>
+      <c r="T26" s="1">
+        <v>3</v>
+      </c>
+      <c r="U26" s="1">
+        <v>4</v>
+      </c>
+      <c r="V26" s="1">
+        <v>5</v>
+      </c>
+      <c r="W26" s="1">
+        <v>6</v>
+      </c>
+      <c r="X26" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="18:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R27" s="1">
+        <v>2</v>
+      </c>
+      <c r="S27" s="1">
+        <v>3</v>
+      </c>
+      <c r="T27" s="1">
+        <v>4</v>
+      </c>
+      <c r="U27" s="1">
+        <v>5</v>
+      </c>
+      <c r="V27" s="1">
+        <v>6</v>
+      </c>
+      <c r="W27" s="1">
+        <v>7</v>
+      </c>
+      <c r="X27" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="18:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R30" s="1">
+        <v>1</v>
+      </c>
+      <c r="S30" s="1">
+        <v>2</v>
+      </c>
+      <c r="T30" s="1">
+        <v>3</v>
+      </c>
+      <c r="U30" s="1">
+        <v>4</v>
+      </c>
+      <c r="V30" s="1">
+        <v>5</v>
+      </c>
+      <c r="W30" s="1">
+        <v>6</v>
+      </c>
+      <c r="X30" s="1">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37088839-E95D-4540-8E75-5DA4D1D1AB0E}">
+  <dimension ref="F5:N36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N36" sqref="L36:N36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="4.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="6:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1">
+        <v>3</v>
+      </c>
+      <c r="J5" s="1">
+        <v>4</v>
+      </c>
+      <c r="K5" s="1">
+        <v>5</v>
+      </c>
+      <c r="L5" s="1">
+        <v>6</v>
+      </c>
+      <c r="M5" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="6:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1">
+        <v>4</v>
+      </c>
+      <c r="J6" s="1">
+        <v>5</v>
+      </c>
+      <c r="K6" s="1">
+        <v>6</v>
+      </c>
+      <c r="L6" s="1">
+        <v>7</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="6:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="6:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3</v>
+      </c>
+      <c r="J10" s="1">
+        <v>4</v>
+      </c>
+      <c r="K10" s="1">
+        <v>5</v>
+      </c>
+      <c r="L10" s="1">
+        <v>6</v>
+      </c>
+      <c r="M10" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="6:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3</v>
+      </c>
+      <c r="I11" s="1">
+        <v>4</v>
+      </c>
+      <c r="J11" s="1">
+        <v>5</v>
+      </c>
+      <c r="K11" s="1">
+        <v>6</v>
+      </c>
+      <c r="L11" s="1">
+        <v>7</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="6:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="6:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2</v>
+      </c>
+      <c r="I15" s="1">
+        <v>3</v>
+      </c>
+      <c r="J15" s="1">
+        <v>4</v>
+      </c>
+      <c r="K15" s="1">
+        <v>5</v>
+      </c>
+      <c r="L15" s="1">
+        <v>6</v>
+      </c>
+      <c r="M15" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="6:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>3</v>
+      </c>
+      <c r="I16" s="1">
+        <v>4</v>
+      </c>
+      <c r="J16" s="1">
+        <v>5</v>
+      </c>
+      <c r="K16" s="1">
+        <v>6</v>
+      </c>
+      <c r="L16" s="1">
+        <v>7</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="6:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="6:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1">
+        <v>2</v>
+      </c>
+      <c r="I19" s="1">
+        <v>3</v>
+      </c>
+      <c r="J19" s="1">
+        <v>4</v>
+      </c>
+      <c r="K19" s="1">
+        <v>5</v>
+      </c>
+      <c r="L19" s="1">
+        <v>6</v>
+      </c>
+      <c r="M19" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="6:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>3</v>
+      </c>
+      <c r="I20" s="1">
+        <v>4</v>
+      </c>
+      <c r="J20" s="1">
+        <v>5</v>
+      </c>
+      <c r="K20" s="1">
+        <v>6</v>
+      </c>
+      <c r="L20" s="1">
+        <v>7</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="6:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="6:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1">
+        <v>2</v>
+      </c>
+      <c r="I23" s="1">
+        <v>3</v>
+      </c>
+      <c r="J23" s="1">
+        <v>4</v>
+      </c>
+      <c r="K23" s="1">
+        <v>5</v>
+      </c>
+      <c r="L23" s="1">
+        <v>6</v>
+      </c>
+      <c r="M23" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="6:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <v>3</v>
+      </c>
+      <c r="I24" s="1">
+        <v>4</v>
+      </c>
+      <c r="J24" s="1">
+        <v>5</v>
+      </c>
+      <c r="K24" s="1">
+        <v>6</v>
+      </c>
+      <c r="L24" s="1">
+        <v>7</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="6:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="6:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1">
+        <v>2</v>
+      </c>
+      <c r="I28" s="1">
+        <v>3</v>
+      </c>
+      <c r="J28" s="1">
+        <v>4</v>
+      </c>
+      <c r="K28" s="1">
+        <v>5</v>
+      </c>
+      <c r="L28" s="1">
+        <v>6</v>
+      </c>
+      <c r="M28" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="6:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="1">
+        <v>4</v>
+      </c>
+      <c r="J29" s="1">
+        <v>5</v>
+      </c>
+      <c r="K29" s="1">
+        <v>6</v>
+      </c>
+      <c r="L29" s="1">
+        <v>7</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="6:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="6:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1</v>
+      </c>
+      <c r="H34" s="1">
+        <v>2</v>
+      </c>
+      <c r="I34" s="1">
+        <v>3</v>
+      </c>
+      <c r="J34" s="1">
+        <v>4</v>
+      </c>
+      <c r="K34" s="1">
+        <v>5</v>
+      </c>
+      <c r="L34" s="1">
+        <v>6</v>
+      </c>
+      <c r="M34" s="1">
+        <v>7</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="6:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="1">
+        <v>4</v>
+      </c>
+      <c r="J35" s="1">
+        <v>5</v>
+      </c>
+      <c r="K35" s="1">
+        <v>6</v>
+      </c>
+      <c r="L35" s="1">
+        <v>7</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="6:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>